<commit_message>
A commit from my local computer
</commit_message>
<xml_diff>
--- a/ABC_input/OysterAssociates_final_20Dec2022.xlsx
+++ b/ABC_input/OysterAssociates_final_20Dec2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sotkae/Dropbox/Documents/Publications/CURRENT/gigas-popgen/popgen-OysterAssociates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sotkae/Dropbox/Documents/Publications/CURRENT/gigas-popgen/github/gigas-popgen/ABC_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C05F9C-A91D-D945-81C9-4E1387E5CF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5481B7B-4C4C-9948-847E-73957C148DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-380" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{346D2514-B995-BD42-B27E-031A55FF43A5}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="16440" xr2:uid="{346D2514-B995-BD42-B27E-031A55FF43A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Spp" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="325">
   <si>
     <t>Genus-species</t>
   </si>
@@ -961,9 +961,6 @@
     <t>Asian shore crab</t>
   </si>
   <si>
-    <t>***GENBANK FROM ALLAN</t>
-  </si>
-  <si>
     <t>Cribrilina mutabilis</t>
   </si>
   <si>
@@ -1013,6 +1010,9 @@
   </si>
   <si>
     <t>Palaemon macrodactylus</t>
+  </si>
+  <si>
+    <t>***PHYLOGATR for German samples</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1175,33 +1175,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1217,16 +1198,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1234,7 +1211,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1575,14 +1552,14 @@
   <dimension ref="A1:N71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.1640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="35.1640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -1592,14 +1569,14 @@
     <col min="8" max="8" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="44" style="3" customWidth="1"/>
     <col min="13" max="13" width="20.6640625" style="3" customWidth="1"/>
     <col min="14" max="14" width="59.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1629,21 +1606,21 @@
       <c r="J1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="8" t="s">
         <v>91</v>
       </c>
       <c r="H2" s="4">
@@ -1663,34 +1640,31 @@
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>2005</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="8">
+      <c r="H3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" s="4">
         <v>0.85</v>
       </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="3" t="s">
         <v>303</v>
       </c>
       <c r="N3" t="s">
@@ -1701,34 +1675,30 @@
       <c r="A4" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>2005</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="8">
+      <c r="H4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" s="4">
         <v>0.68</v>
       </c>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
       <c r="N4" t="s">
         <v>59</v>
       </c>
@@ -1737,40 +1707,36 @@
       <c r="A5" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>2005</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="8">
+      <c r="H5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="4">
         <v>0.68</v>
       </c>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
       <c r="N5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="22" t="s">
         <v>232</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1788,8 +1754,8 @@
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>316</v>
+      <c r="G6" s="17" t="s">
+        <v>315</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>83</v>
@@ -1800,7 +1766,7 @@
       <c r="J6" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="4">
         <v>0.89</v>
       </c>
       <c r="N6" t="s">
@@ -1811,36 +1777,33 @@
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>2020</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="8">
+      <c r="H7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="4">
         <v>1</v>
       </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
       <c r="N7" t="s">
         <v>56</v>
       </c>
@@ -1849,36 +1812,34 @@
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>2013</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="8">
+      <c r="H8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="4">
         <v>0.65</v>
       </c>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25" t="s">
+      <c r="M8" s="3" t="s">
         <v>302</v>
       </c>
       <c r="N8" t="s">
@@ -1904,19 +1865,19 @@
       <c r="F9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>31</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="4">
         <v>0.5</v>
       </c>
-      <c r="L9" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="M9" s="11" t="s">
+      <c r="L9" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="M9" s="6" t="s">
         <v>306</v>
       </c>
       <c r="N9" t="s">
@@ -1927,35 +1888,31 @@
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>2018</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="8">
+      <c r="I10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="4">
         <v>0.46</v>
       </c>
-      <c r="L10" s="11" t="s">
-        <v>307</v>
-      </c>
+      <c r="L10" s="6"/>
       <c r="N10" t="s">
         <v>41</v>
       </c>
@@ -1964,36 +1921,34 @@
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>2018</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="8">
+      <c r="H11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="4">
         <v>0.73</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="L11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="M11" s="10"/>
+      <c r="M11" s="6"/>
       <c r="N11" t="s">
         <v>54</v>
       </c>
@@ -2002,40 +1957,40 @@
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>2006</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="8">
+      <c r="H12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K12" s="4">
         <v>0.76</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="M12" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>301</v>
       </c>
       <c r="N12" t="s">
@@ -2046,22 +2001,22 @@
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>2018</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="4" t="s">
@@ -2073,14 +2028,13 @@
       <c r="J14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="4">
         <v>0.48</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M14" s="10"/>
-      <c r="N14" s="9"/>
+      <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -2101,17 +2055,17 @@
       <c r="F15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="4">
         <v>0.56000000000000005</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>305</v>
@@ -2122,7 +2076,7 @@
     </row>
     <row r="16" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>77</v>
@@ -2148,9 +2102,9 @@
       <c r="I16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K16" s="32"/>
+      <c r="K16" s="23"/>
       <c r="L16" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>300</v>
@@ -2159,22 +2113,10 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="9" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -2201,7 +2143,7 @@
       <c r="H18" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="K18" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L18" s="3" t="s">
@@ -2233,16 +2175,16 @@
       <c r="I19" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="K19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L19" s="13" t="s">
+      <c r="L19" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="M19" s="13"/>
-    </row>
-    <row r="20" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="M19" s="6"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -2263,23 +2205,18 @@
       <c r="G20" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="M20" s="3"/>
-      <c r="N20"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2305,7 +2242,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -2329,7 +2266,7 @@
       <c r="H22" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="K22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L22" s="3" t="s">
@@ -2340,7 +2277,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="6" t="s">
         <v>217</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2364,7 +2301,7 @@
       <c r="J23" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K23" s="7" t="s">
+      <c r="K23" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L23" s="3" t="s">
@@ -2372,10 +2309,10 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="16" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -2398,7 +2335,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -2419,7 +2356,7 @@
       <c r="G25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L25" s="3" t="s">
@@ -2451,7 +2388,7 @@
       <c r="H26" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="K26" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L26" s="3" t="s">
@@ -2459,20 +2396,20 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
-        <v>308</v>
+      <c r="A27" s="18" t="s">
+        <v>307</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>157</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D27" s="4">
         <v>2020</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>14</v>
@@ -2491,7 +2428,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="6" t="s">
         <v>285</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -2509,7 +2446,7 @@
       <c r="F28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H28" s="4" t="s">
@@ -2520,7 +2457,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -2544,7 +2481,7 @@
       <c r="H29" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K29" s="7" t="s">
+      <c r="K29" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L29" s="3" t="s">
@@ -2552,10 +2489,10 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -2602,7 +2539,7 @@
       <c r="F31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="24"/>
+      <c r="G31" s="17"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -2621,7 +2558,7 @@
         <v>69</v>
       </c>
       <c r="F32" s="1"/>
-      <c r="G32" s="24"/>
+      <c r="G32" s="17"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -2654,7 +2591,7 @@
       <c r="J33" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K33" s="7" t="s">
+      <c r="K33" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L33" s="3" t="s">
@@ -2662,10 +2599,10 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="16" t="s">
         <v>192</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -2694,7 +2631,7 @@
       <c r="A35" t="s">
         <v>238</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="16" t="s">
         <v>237</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -2723,10 +2660,10 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -2755,7 +2692,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="18" t="s">
         <v>255</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2784,7 +2721,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
+      <c r="A38" t="s">
         <v>239</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2806,27 +2743,27 @@
         <v>83</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="N38" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="13" t="s">
-        <v>321</v>
-      </c>
-      <c r="B39" s="23" t="s">
+      <c r="A39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B39" s="16" t="s">
         <v>284</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D39" s="4">
         <v>2020</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>14</v>
@@ -2842,7 +2779,7 @@
       <c r="A40" t="s">
         <v>152</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -2865,10 +2802,10 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -2888,10 +2825,10 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -2911,10 +2848,10 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -2940,7 +2877,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -2961,7 +2898,7 @@
       <c r="G44" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="K44" s="7" t="s">
+      <c r="K44" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L44" s="3" t="s">
@@ -2969,7 +2906,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -2990,7 +2927,7 @@
       <c r="G45" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K45" s="7" t="s">
+      <c r="K45" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L45" s="3" t="s">
@@ -2998,7 +2935,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -3025,7 +2962,7 @@
       <c r="I46" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K46" s="7" t="s">
+      <c r="K46" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L46" s="3" t="s">
@@ -3036,7 +2973,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -3063,7 +3000,7 @@
       <c r="I47" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K47" s="7" t="s">
+      <c r="K47" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L47" s="3" t="s">
@@ -3074,7 +3011,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -3101,7 +3038,7 @@
       <c r="I48" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K48" s="7" t="s">
+      <c r="K48" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L48" s="3" t="s">
@@ -3112,7 +3049,7 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -3139,7 +3076,7 @@
       <c r="I49" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K49" s="7" t="s">
+      <c r="K49" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L49" s="3" t="s">
@@ -3150,10 +3087,10 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="B50" s="23" t="s">
+      <c r="B50" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -3174,13 +3111,13 @@
       <c r="H50" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L50" s="29" t="s">
+      <c r="L50" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="M50" s="29"/>
+      <c r="M50" s="20"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="6" t="s">
         <v>86</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -3201,7 +3138,7 @@
       <c r="G51" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K51" s="7" t="s">
+      <c r="K51" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L51" s="3" t="s">
@@ -3209,7 +3146,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="6" t="s">
         <v>86</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -3230,7 +3167,7 @@
       <c r="G52" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K52" s="7" t="s">
+      <c r="K52" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L52" s="3" t="s">
@@ -3238,7 +3175,7 @@
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="6" t="s">
         <v>100</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -3262,7 +3199,7 @@
       <c r="H53" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K53" s="7" t="s">
+      <c r="K53" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L53" s="3" t="s">
@@ -3270,7 +3207,7 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="6" t="s">
         <v>100</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -3291,7 +3228,7 @@
       <c r="G54" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="K54" s="7" t="s">
+      <c r="K54" s="4" t="s">
         <v>41</v>
       </c>
       <c r="L54" s="3" t="s">
@@ -3299,10 +3236,10 @@
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="B55" s="23" t="s">
+      <c r="B55" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -3331,7 +3268,7 @@
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -3357,16 +3294,16 @@
       </c>
     </row>
     <row r="57" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="23"/>
+      <c r="B57" s="16"/>
       <c r="C57" s="3"/>
     </row>
     <row r="58" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
-        <v>314</v>
+      <c r="A58" s="8" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -3409,7 +3346,7 @@
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -3426,7 +3363,7 @@
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="6" t="s">
         <v>92</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -3467,7 +3404,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>11</v>
@@ -3485,18 +3422,18 @@
         <v>14</v>
       </c>
       <c r="G64" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L64" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="H64" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="L64" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A65" s="15" t="s">
-        <v>313</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>11</v>
@@ -3513,7 +3450,7 @@
       <c r="F65" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="5" t="s">
+      <c r="G65" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H65" s="4" t="s">
@@ -3527,18 +3464,18 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A66" s="27" t="s">
+      <c r="A66" s="19" t="s">
         <v>253</v>
       </c>
       <c r="B66" s="1"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="6" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="6" t="s">
         <v>256</v>
       </c>
     </row>
@@ -3553,7 +3490,7 @@
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="6" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3566,7 +3503,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:N12">
     <sortCondition ref="A3:A12"/>
   </sortState>
-  <conditionalFormatting sqref="L19:M19 H3:J12 H14:J65">
+  <conditionalFormatting sqref="H3:J12 H14:J65 L19:M19">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",H3)))</formula>
     </cfRule>
@@ -3590,56 +3527,56 @@
   <sheetData>
     <row r="2" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="15" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="10" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="10" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="10" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="12" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+      <c r="A8" s="14"/>
     </row>
     <row r="10" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="9" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="11" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="11" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="11" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="11" t="s">
         <v>265</v>
       </c>
     </row>
@@ -3649,22 +3586,22 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="11" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="11" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="13" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
+      <c r="A20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3682,9 +3619,9 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="12"/>
+      <c r="A1" s="7"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="13"/>
+      <c r="C1" s="6"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -3692,15 +3629,15 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="7"/>
+      <c r="K1" s="4"/>
       <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="19" t="s">
         <v>258</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="13"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -3708,15 +3645,15 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="7"/>
+      <c r="K2" s="4"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="6" t="s">
         <v>257</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="13"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -3724,11 +3661,11 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="7"/>
+      <c r="K3" s="4"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="6" t="s">
         <v>261</v>
       </c>
       <c r="B4" s="1"/>
@@ -3740,11 +3677,11 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="7"/>
+      <c r="K4" s="4"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="6" t="s">
         <v>262</v>
       </c>
       <c r="B5" s="1"/>
@@ -3756,11 +3693,11 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="7"/>
+      <c r="K5" s="4"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="6" t="s">
         <v>263</v>
       </c>
       <c r="B6" s="1"/>
@@ -3772,11 +3709,11 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="7"/>
+      <c r="K6" s="4"/>
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -3786,7 +3723,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="7"/>
+      <c r="K7" s="4"/>
       <c r="L7" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -3799,7 +3736,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="7"/>
+      <c r="K9" s="4"/>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -3812,7 +3749,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="7"/>
+      <c r="K10" s="4"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3825,11 +3762,11 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="7"/>
+      <c r="K11" s="4"/>
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="8" t="s">
         <v>96</v>
       </c>
       <c r="B12" s="4"/>
@@ -3841,11 +3778,11 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="7"/>
+      <c r="K12" s="4"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -3867,11 +3804,11 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="7"/>
+      <c r="K13" s="4"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -3893,17 +3830,17 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="7"/>
+      <c r="K14" s="4"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="16" t="s">
         <v>223</v>
       </c>
       <c r="D15" s="1">
@@ -3917,17 +3854,17 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="7"/>
+      <c r="K15" s="4"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>234</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="16" t="s">
         <v>189</v>
       </c>
       <c r="D16" s="1">
@@ -3941,11 +3878,11 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="7"/>
+      <c r="K16" s="4"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="7" t="s">
         <v>155</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3967,17 +3904,17 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="7"/>
+      <c r="K17" s="4"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="23" t="s">
+      <c r="B18" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>127</v>
       </c>
       <c r="D18" s="1">
@@ -3993,13 +3930,13 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="7"/>
+      <c r="K18" s="4"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -4007,13 +3944,13 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="7"/>
+      <c r="K19" s="4"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -4021,13 +3958,13 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="7"/>
+      <c r="K20" s="4"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -4035,13 +3972,13 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="7"/>
+      <c r="K21" s="4"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="23"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -4049,14 +3986,14 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="7"/>
+      <c r="K22" s="4"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="B23" s="23"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -4065,7 +4002,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="7"/>
+      <c r="K23" s="4"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -4087,27 +4024,27 @@
       <c r="F24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="24" t="s">
+      <c r="G24" s="17" t="s">
         <v>229</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="7"/>
+      <c r="K24" s="4"/>
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="24"/>
+      <c r="G25" s="17"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="7"/>
+      <c r="K25" s="4"/>
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -4116,11 +4053,11 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="24"/>
+      <c r="G26" s="17"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="7"/>
+      <c r="K26" s="4"/>
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -4129,11 +4066,11 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="24"/>
+      <c r="G27" s="17"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="7"/>
+      <c r="K27" s="4"/>
       <c r="L27" s="3"/>
     </row>
     <row r="28" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4142,15 +4079,15 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="24"/>
+      <c r="G28" s="17"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="7"/>
+      <c r="K28" s="4"/>
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="8" t="s">
         <v>236</v>
       </c>
       <c r="B29" s="1"/>
@@ -4162,7 +4099,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="7"/>
+      <c r="K29" s="4"/>
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -4172,7 +4109,7 @@
       <c r="B30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="23"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -4180,14 +4117,14 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="7"/>
+      <c r="K30" s="4"/>
       <c r="L30" s="3"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>242</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="16" t="s">
         <v>192</v>
       </c>
       <c r="C31" t="s">
@@ -4204,14 +4141,14 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="7"/>
+      <c r="K31" s="4"/>
       <c r="L31" s="3"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>242</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="16" t="s">
         <v>192</v>
       </c>
       <c r="C32" t="s">
@@ -4228,11 +4165,11 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="7"/>
+      <c r="K32" s="4"/>
       <c r="L32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B33" s="23"/>
+      <c r="B33" s="16"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -4240,11 +4177,11 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="7"/>
+      <c r="K33" s="4"/>
       <c r="L33" s="3"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B34" s="23"/>
+      <c r="B34" s="16"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -4252,7 +4189,7 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="7"/>
+      <c r="K34" s="4"/>
       <c r="L34" s="3"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -4261,764 +4198,764 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B36" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="12"/>
+      <c r="B36" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B37" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="12"/>
+      <c r="B37" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="7"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B38" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="12"/>
+      <c r="B38" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="7"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B39" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="23" t="s">
+      <c r="B39" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="12"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="7"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="12"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="7"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="B41" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="12"/>
+      <c r="B41" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="7"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="12"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="7"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B43" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="30"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="12"/>
+      <c r="B43" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="16"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="7"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B44" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="12"/>
+      <c r="B44" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="7"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="12"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="12"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="7"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="12"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="7"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B48" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="23"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="12"/>
+      <c r="B48" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="16"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="7"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B49" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="23"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="29"/>
-      <c r="M49" s="12"/>
+      <c r="B49" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="16"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="7"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B50" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="30"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="30"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="12"/>
+      <c r="B50" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="7"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B51" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="23"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="29"/>
-      <c r="M51" s="12"/>
+      <c r="B51" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="16"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="7"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="12" t="s">
+      <c r="A52" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" s="23"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="30"/>
-      <c r="H52" s="30"/>
-      <c r="I52" s="30"/>
-      <c r="J52" s="30"/>
-      <c r="K52" s="30"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="12"/>
+      <c r="B52" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="16"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="7"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="23" t="s">
+      <c r="B53" s="16"/>
+      <c r="C53" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="D53" s="23">
+      <c r="D53" s="16">
         <v>2017</v>
       </c>
-      <c r="E53" s="23" t="s">
+      <c r="E53" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="23" t="s">
+      <c r="F53" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30"/>
-      <c r="K53" s="30"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="12"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="20"/>
+      <c r="M53" s="7"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B54" s="23"/>
-      <c r="C54" s="23" t="s">
+      <c r="B54" s="16"/>
+      <c r="C54" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="23">
+      <c r="D54" s="16">
         <v>2009</v>
       </c>
-      <c r="E54" s="23" t="s">
+      <c r="E54" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="F54" s="23" t="s">
+      <c r="F54" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="G54" s="30"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="12"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="20"/>
+      <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="B55" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" s="23"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
-      <c r="J55" s="30"/>
-      <c r="K55" s="30"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="12"/>
+      <c r="B55" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="16"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="21"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="7"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="12" t="s">
+      <c r="A56" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B56" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="23"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="30"/>
-      <c r="J56" s="30"/>
-      <c r="K56" s="30"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="12"/>
+      <c r="B56" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="16"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="20"/>
+      <c r="M56" s="7"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="12" t="s">
+      <c r="A57" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B57" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" s="23"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
-      <c r="J57" s="30"/>
-      <c r="K57" s="30"/>
-      <c r="L57" s="29"/>
-      <c r="M57" s="12"/>
+      <c r="B57" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="16"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="7"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B58" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="23"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="30"/>
-      <c r="H58" s="30"/>
-      <c r="I58" s="30"/>
-      <c r="J58" s="30"/>
-      <c r="K58" s="30"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="12"/>
+      <c r="B58" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="16"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="7"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B59" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="23"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="30"/>
-      <c r="I59" s="30"/>
-      <c r="J59" s="30"/>
-      <c r="K59" s="30"/>
-      <c r="L59" s="29"/>
-      <c r="M59" s="12"/>
+      <c r="B59" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="16"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="20"/>
+      <c r="M59" s="7"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="23" t="s">
+      <c r="B60" s="16"/>
+      <c r="C60" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="30"/>
-      <c r="J60" s="30"/>
-      <c r="K60" s="30"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="12"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="7"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="12" t="s">
+      <c r="A61" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B61" s="23"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="30"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="30"/>
-      <c r="K61" s="30"/>
-      <c r="L61" s="29"/>
-      <c r="M61" s="12"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="7"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="30"/>
-      <c r="J62" s="30"/>
-      <c r="K62" s="30"/>
-      <c r="L62" s="29"/>
-      <c r="M62" s="12"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="7"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="23"/>
-      <c r="H63" s="30"/>
-      <c r="I63" s="30"/>
-      <c r="J63" s="30"/>
-      <c r="K63" s="30"/>
-      <c r="L63" s="29"/>
-      <c r="M63" s="12"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="20"/>
+      <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B64" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C64" s="23"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
-      <c r="J64" s="30"/>
-      <c r="K64" s="30"/>
-      <c r="L64" s="29"/>
-      <c r="M64" s="12"/>
+      <c r="B64" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="21"/>
+      <c r="K64" s="21"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="7"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A65" s="12" t="s">
+      <c r="A65" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B65" s="23"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="23"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="30"/>
-      <c r="H65" s="30"/>
-      <c r="I65" s="30"/>
-      <c r="J65" s="30"/>
-      <c r="K65" s="30"/>
-      <c r="L65" s="29"/>
-      <c r="M65" s="12"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="21"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="20"/>
+      <c r="M65" s="7"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B66" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="23"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="30"/>
-      <c r="G66" s="30"/>
-      <c r="H66" s="30"/>
-      <c r="I66" s="30"/>
-      <c r="J66" s="30"/>
-      <c r="K66" s="30"/>
-      <c r="L66" s="29"/>
-      <c r="M66" s="12"/>
+      <c r="B66" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="16"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="7"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A67" s="12" t="s">
+      <c r="A67" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B67" s="30"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
-      <c r="G67" s="30"/>
-      <c r="H67" s="30"/>
-      <c r="I67" s="30"/>
-      <c r="J67" s="30"/>
-      <c r="K67" s="30"/>
-      <c r="L67" s="29"/>
-      <c r="M67" s="12"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="20"/>
+      <c r="M67" s="7"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A68" s="12" t="s">
+      <c r="A68" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B68" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C68" s="23"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
-      <c r="G68" s="30"/>
-      <c r="H68" s="30"/>
-      <c r="I68" s="30"/>
-      <c r="J68" s="30"/>
-      <c r="K68" s="30"/>
-      <c r="L68" s="29"/>
-      <c r="M68" s="12"/>
+      <c r="B68" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="16"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="20"/>
+      <c r="M68" s="7"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A69" s="12" t="s">
+      <c r="A69" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B69" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69" s="23"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
-      <c r="G69" s="30"/>
-      <c r="H69" s="30"/>
-      <c r="I69" s="30"/>
-      <c r="J69" s="30"/>
-      <c r="K69" s="30"/>
-      <c r="L69" s="29"/>
-      <c r="M69" s="12"/>
+      <c r="B69" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="16"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="20"/>
+      <c r="M69" s="7"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A70" s="12" t="s">
+      <c r="A70" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B70" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" s="23"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="30"/>
-      <c r="G70" s="30"/>
-      <c r="H70" s="30"/>
-      <c r="I70" s="30"/>
-      <c r="J70" s="30"/>
-      <c r="K70" s="30"/>
-      <c r="L70" s="29"/>
-      <c r="M70" s="12"/>
+      <c r="B70" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="16"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="20"/>
+      <c r="M70" s="7"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B71" s="23"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23"/>
-      <c r="G71" s="30"/>
-      <c r="H71" s="30"/>
-      <c r="I71" s="30"/>
-      <c r="J71" s="30"/>
-      <c r="K71" s="30"/>
-      <c r="L71" s="29"/>
-      <c r="M71" s="12"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="20"/>
+      <c r="M71" s="7"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A72" s="12" t="s">
+      <c r="A72" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B72" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C72" s="23" t="s">
+      <c r="B72" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="30"/>
-      <c r="G72" s="30"/>
-      <c r="H72" s="30"/>
-      <c r="I72" s="30"/>
-      <c r="J72" s="30"/>
-      <c r="K72" s="30"/>
-      <c r="L72" s="29"/>
-      <c r="M72" s="12"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
+      <c r="J72" s="21"/>
+      <c r="K72" s="21"/>
+      <c r="L72" s="20"/>
+      <c r="M72" s="7"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B73" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C73" s="23"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
-      <c r="G73" s="30"/>
-      <c r="H73" s="30"/>
-      <c r="I73" s="30"/>
-      <c r="J73" s="30"/>
-      <c r="K73" s="30"/>
-      <c r="L73" s="29"/>
-      <c r="M73" s="12"/>
+      <c r="B73" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="16"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="20"/>
+      <c r="M73" s="7"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A74" s="12" t="s">
+      <c r="A74" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B74" s="23" t="s">
+      <c r="B74" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="30"/>
-      <c r="H74" s="30"/>
-      <c r="I74" s="30"/>
-      <c r="J74" s="30"/>
-      <c r="K74" s="30"/>
-      <c r="L74" s="29"/>
-      <c r="M74" s="12"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="20"/>
+      <c r="M74" s="7"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A75" s="12" t="s">
+      <c r="A75" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B75" s="30" t="s">
+      <c r="B75" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="C75" s="23" t="s">
+      <c r="C75" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="D75" s="30">
+      <c r="D75" s="21">
         <v>2005</v>
       </c>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
-      <c r="G75" s="30"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="30"/>
-      <c r="J75" s="30"/>
-      <c r="K75" s="30"/>
-      <c r="L75" s="29"/>
-      <c r="M75" s="12"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="20"/>
+      <c r="M75" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H9:J34">

</xml_diff>